<commit_message>
update to replication report
</commit_message>
<xml_diff>
--- a/GroupB_6-7-2014/data/S1_Subway.xlsx
+++ b/GroupB_6-7-2014/data/S1_Subway.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crazy\OneDrive\Desktop\reproducibility_assignment\GroupB_6-7-2014\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_E0551DFBD43F6F40150868432EDBC42CF882E354" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21520" yWindow="3000" windowWidth="26700" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,8 +66,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -465,18 +471,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="20.3125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.3125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>